<commit_message>
Scroll up con javascript
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Data.xlsx
+++ b/src/main/resources/Data/Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="48">
   <si>
     <t>Nombre</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Aire Acondicionado 12.000BTU 2 HYUNDAI HY12K229IVGF</t>
+  </si>
+  <si>
+    <t>Encuentra Tu Persona Vitamina PLANETA 3028371</t>
+  </si>
+  <si>
+    <t>Primeros Mil Días Del Bebe GRIJALBO 1303320</t>
+  </si>
+  <si>
+    <t>Cree En Ti DIANA 3026463</t>
   </si>
 </sst>
 </file>
@@ -535,7 +544,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -543,15 +552,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>

</xml_diff>